<commit_message>
little mistake that was causing dmacgenformdef to not work
</commit_message>
<xml_diff>
--- a/app/config/tables/distribution/forms/set_is_distributed/set_is_distributed.xlsx
+++ b/app/config/tables/distribution/forms/set_is_distributed/set_is_distributed.xlsx
@@ -1014,7 +1014,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1034,7 +1034,7 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="26" t="b">
+      <c r="B2" s="26">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -1045,7 +1045,7 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="26" t="b">
+      <c r="B3" s="26">
         <v>0</v>
       </c>
       <c r="C3" t="s">

</xml_diff>